<commit_message>
Actualización de cronograma de actividades
</commit_message>
<xml_diff>
--- a/Desarrollo/SMZR/Gestión/SMZR_CA.xlsx
+++ b/Desarrollo/SMZR/Gestión/SMZR_CA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MORALES\Desktop\RebroteSolution\Desarrollo\SMZR\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rubi/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0ED0CA2-5C30-49C8-85DA-E991886D8284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D2F14DF-2C58-B446-963C-045ADB35AD73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -237,7 +237,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,8 +298,59 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Nunito Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Nunito Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Nunito Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Nunito Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Nunito Regular"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,6 +405,21 @@
         <bgColor rgb="FF9FC5E8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -403,10 +469,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -550,8 +619,26 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="14" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="12" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="11" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -767,33 +854,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.625" customWidth="1"/>
-    <col min="2" max="2" width="39.625" customWidth="1"/>
-    <col min="3" max="3" width="11.625" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="15.875" customWidth="1"/>
-    <col min="6" max="6" width="22.375" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
     <col min="7" max="7" width="14.5" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="5.625" customWidth="1"/>
-    <col min="10" max="10" width="5.125" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" customWidth="1"/>
+    <col min="10" max="10" width="5.1640625" customWidth="1"/>
     <col min="11" max="11" width="5" customWidth="1"/>
-    <col min="12" max="18" width="4.875" customWidth="1"/>
-    <col min="19" max="20" width="5.375" customWidth="1"/>
+    <col min="12" max="18" width="4.83203125" customWidth="1"/>
+    <col min="19" max="20" width="5.33203125" customWidth="1"/>
     <col min="21" max="25" width="5" customWidth="1"/>
-    <col min="26" max="27" width="5.375" customWidth="1"/>
-    <col min="28" max="29" width="5.125" customWidth="1"/>
+    <col min="26" max="27" width="5.33203125" customWidth="1"/>
+    <col min="28" max="29" width="5.1640625" customWidth="1"/>
     <col min="30" max="31" width="4.5" customWidth="1"/>
-    <col min="32" max="36" width="4.375" customWidth="1"/>
-    <col min="37" max="40" width="5.125" customWidth="1"/>
-    <col min="41" max="43" width="5.875" customWidth="1"/>
-    <col min="44" max="49" width="9.375" customWidth="1"/>
+    <col min="32" max="36" width="4.33203125" customWidth="1"/>
+    <col min="37" max="40" width="5.1640625" customWidth="1"/>
+    <col min="41" max="43" width="5.83203125" customWidth="1"/>
+    <col min="44" max="49" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="78" customHeight="1">
@@ -952,7 +1039,7 @@
       <c r="F2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="49">
         <v>1</v>
       </c>
       <c r="H2" s="12" t="s">
@@ -1015,7 +1102,7 @@
       <c r="F3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="49">
         <v>1</v>
       </c>
       <c r="H3" s="12" t="s">
@@ -1078,7 +1165,7 @@
       <c r="F4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="49">
         <v>1</v>
       </c>
       <c r="H4" s="12" t="s">
@@ -1141,7 +1228,7 @@
       <c r="F5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="49">
         <v>1</v>
       </c>
       <c r="H5" s="12" t="s">
@@ -1204,7 +1291,7 @@
       <c r="F6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="49">
         <v>1</v>
       </c>
       <c r="H6" s="12" t="s">
@@ -1267,7 +1354,7 @@
       <c r="F7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="49">
         <v>1</v>
       </c>
       <c r="H7" s="12" t="s">
@@ -1330,7 +1417,7 @@
       <c r="F8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="49">
         <v>1</v>
       </c>
       <c r="H8" s="12" t="s">
@@ -1393,7 +1480,7 @@
       <c r="F9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="49">
         <v>1</v>
       </c>
       <c r="H9" s="12" t="s">
@@ -1456,7 +1543,7 @@
       <c r="F10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="49">
         <v>1</v>
       </c>
       <c r="H10" s="12" t="s">
@@ -1519,7 +1606,7 @@
       <c r="F11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="49">
         <v>1</v>
       </c>
       <c r="H11" s="12" t="s">
@@ -1578,7 +1665,7 @@
         <v>44029</v>
       </c>
       <c r="F12" s="24"/>
-      <c r="G12" s="25">
+      <c r="G12" s="50">
         <v>1</v>
       </c>
       <c r="H12" s="26"/>
@@ -1639,7 +1726,7 @@
       <c r="F13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="49">
         <v>1</v>
       </c>
       <c r="H13" s="12" t="s">
@@ -1702,7 +1789,7 @@
       <c r="F14" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="49">
         <v>1</v>
       </c>
       <c r="H14" s="12" t="s">
@@ -1760,12 +1847,12 @@
         <v>44032</v>
       </c>
       <c r="E15" s="9">
-        <v>44055</v>
+        <v>44062</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="51">
         <v>0.8</v>
       </c>
       <c r="H15" s="12" t="s">
@@ -1795,8 +1882,8 @@
       <c r="AD15" s="32"/>
       <c r="AE15" s="32"/>
       <c r="AF15" s="32"/>
-      <c r="AG15" s="17"/>
-      <c r="AH15" s="17"/>
+      <c r="AG15" s="21"/>
+      <c r="AH15" s="21"/>
       <c r="AI15" s="17"/>
       <c r="AJ15" s="18"/>
       <c r="AK15" s="17"/>
@@ -1828,7 +1915,7 @@
       <c r="F16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="49">
         <v>1</v>
       </c>
       <c r="H16" s="12" t="s">
@@ -1886,13 +1973,13 @@
         <v>44035</v>
       </c>
       <c r="E17" s="9">
-        <v>44057</v>
+        <v>44059</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="11">
-        <v>0.8</v>
+      <c r="G17" s="51">
+        <v>0.9</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>35</v>
@@ -1921,7 +2008,7 @@
       <c r="AD17" s="21"/>
       <c r="AE17" s="21"/>
       <c r="AF17" s="21"/>
-      <c r="AG17" s="17"/>
+      <c r="AG17" s="21"/>
       <c r="AH17" s="17"/>
       <c r="AI17" s="17"/>
       <c r="AJ17" s="18"/>
@@ -1954,8 +2041,8 @@
       <c r="F18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="11">
-        <v>0.1</v>
+      <c r="G18" s="51">
+        <v>0.3</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>35</v>
@@ -2012,13 +2099,13 @@
         <v>44035</v>
       </c>
       <c r="E19" s="9">
-        <v>44057</v>
+        <v>44062</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="11">
-        <v>0.1</v>
+      <c r="G19" s="51">
+        <v>0.2</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>35</v>
@@ -2047,8 +2134,8 @@
       <c r="AD19" s="21"/>
       <c r="AE19" s="21"/>
       <c r="AF19" s="21"/>
-      <c r="AG19" s="30"/>
-      <c r="AH19" s="30"/>
+      <c r="AG19" s="21"/>
+      <c r="AH19" s="21"/>
       <c r="AI19" s="17"/>
       <c r="AJ19" s="18"/>
       <c r="AK19" s="17"/>
@@ -2080,7 +2167,7 @@
       <c r="F20" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="49">
         <v>1</v>
       </c>
       <c r="H20" s="12" t="s">
@@ -2143,8 +2230,8 @@
       <c r="F21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="11">
-        <v>0.2</v>
+      <c r="G21" s="51">
+        <v>0.5</v>
       </c>
       <c r="H21" s="36" t="s">
         <v>41</v>
@@ -2172,9 +2259,9 @@
       <c r="AC21" s="21"/>
       <c r="AD21" s="21"/>
       <c r="AE21" s="21"/>
-      <c r="AF21" s="30"/>
-      <c r="AG21" s="30"/>
-      <c r="AH21" s="30"/>
+      <c r="AF21" s="21"/>
+      <c r="AG21" s="21"/>
+      <c r="AH21" s="21"/>
       <c r="AI21" s="30"/>
       <c r="AJ21" s="33"/>
       <c r="AK21" s="30"/>
@@ -2202,7 +2289,7 @@
         <v>44063</v>
       </c>
       <c r="F22" s="24"/>
-      <c r="G22" s="40">
+      <c r="G22" s="52">
         <v>0</v>
       </c>
       <c r="H22" s="41"/>
@@ -2263,7 +2350,7 @@
       <c r="F23" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="49">
         <v>0.1</v>
       </c>
       <c r="H23" s="36" t="s">
@@ -2326,7 +2413,7 @@
       <c r="F24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="35">
+      <c r="G24" s="53">
         <v>0</v>
       </c>
       <c r="H24" s="36" t="s">
@@ -2389,7 +2476,7 @@
       <c r="F25" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="35">
+      <c r="G25" s="53">
         <v>0</v>
       </c>
       <c r="H25" s="36" t="s">
@@ -2452,7 +2539,7 @@
       <c r="F26" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="35">
+      <c r="G26" s="53">
         <v>0</v>
       </c>
       <c r="H26" s="44" t="s">
@@ -2511,7 +2598,7 @@
         <v>44066</v>
       </c>
       <c r="F27" s="24"/>
-      <c r="G27" s="40">
+      <c r="G27" s="52">
         <v>0</v>
       </c>
       <c r="H27" s="41"/>
@@ -2572,7 +2659,7 @@
       <c r="F28" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="35">
+      <c r="G28" s="53">
         <v>0</v>
       </c>
       <c r="H28" s="36" t="s">
@@ -2635,7 +2722,7 @@
       <c r="F29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="35">
+      <c r="G29" s="53">
         <v>0</v>
       </c>
       <c r="H29" s="36" t="s">
@@ -2698,7 +2785,7 @@
       <c r="F30" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G30" s="35">
+      <c r="G30" s="53">
         <v>0</v>
       </c>
       <c r="H30" s="36" t="s">
@@ -2761,7 +2848,7 @@
       <c r="F31" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="35">
+      <c r="G31" s="53">
         <v>0</v>
       </c>
       <c r="H31" s="36" t="s">
@@ -2824,7 +2911,7 @@
       <c r="F32" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="35">
+      <c r="G32" s="53">
         <v>0</v>
       </c>
       <c r="H32" s="36" t="s">

</xml_diff>